<commit_message>
GUI: Now using APIs to delete RIPs
</commit_message>
<xml_diff>
--- a/QA/Tests/_Test_Suite_Total_Statistics.xlsx
+++ b/QA/Tests/_Test_Suite_Total_Statistics.xlsx
@@ -421,22 +421,22 @@
             <v>10</v>
           </cell>
           <cell r="G1">
-            <v>4</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="2">
           <cell r="G2">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="4">
           <cell r="G4">
-            <v>55</v>
+            <v>54</v>
           </cell>
         </row>
         <row r="5">
           <cell r="G5">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
       </sheetData>
@@ -799,7 +799,7 @@
       </c>
       <c r="N1" s="7">
         <f>N2/L1</f>
-        <v>0.73809523809523814</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -841,14 +841,14 @@
       </c>
       <c r="L2" s="4">
         <f>SUM($B:$B)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="3">
         <f>SUM(L2:L3)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -890,21 +890,21 @@
       </c>
       <c r="L3" s="4">
         <f>SUM($C:$C)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="7">
         <f>L3/L1</f>
-        <v>0.47619047619047616</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="O3" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="24">
         <f>L3/N2</f>
-        <v>0.64516129032258063</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -951,11 +951,11 @@
       </c>
       <c r="B5" s="9">
         <f>[4]Sheet1!$G$1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="9">
         <f>[4]Sheet1!$G$2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9">
         <f>[4]Sheet1!$E$1</f>
@@ -963,20 +963,20 @@
       </c>
       <c r="E5" s="19">
         <f t="shared" ref="E5" si="2">C5/D5</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="12">
         <f>[4]Sheet1!$G$5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H5" s="9">
         <f>[4]Sheet1!$G$4</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="22">
         <f t="shared" ref="I5" si="3">G5/H5</f>
-        <v>0</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="4" t="s">
@@ -984,7 +984,7 @@
       </c>
       <c r="L5" s="4">
         <f xml:space="preserve"> SUM($H:$H)</f>
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L6" s="4">
         <f xml:space="preserve"> SUM($G:$G)</f>
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="L7" s="7">
         <f>L6/L5</f>
-        <v>0.52117263843648209</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="M7" s="3"/>
     </row>

</xml_diff>

<commit_message>
FUNCTIONALITY: Tagged the newly tested test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/_Test_Suite_Total_Statistics.xlsx
+++ b/QA/Tests/_Test_Suite_Total_Statistics.xlsx
@@ -293,32 +293,32 @@
       <sheetData sheetId="0">
         <row r="1">
           <cell r="H1">
-            <v>28</v>
+            <v>29</v>
           </cell>
         </row>
         <row r="2">
           <cell r="H2">
-            <v>7</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="3">
           <cell r="H3">
-            <v>16</v>
+            <v>18</v>
           </cell>
         </row>
         <row r="5">
           <cell r="H5">
-            <v>213</v>
+            <v>227</v>
           </cell>
         </row>
         <row r="6">
           <cell r="H6">
-            <v>121</v>
+            <v>143</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -436,7 +436,7 @@
         </row>
         <row r="5">
           <cell r="G5">
-            <v>10</v>
+            <v>9</v>
           </cell>
         </row>
       </sheetData>
@@ -737,7 +737,7 @@
   <dimension ref="A1:P175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,14 +792,14 @@
       </c>
       <c r="L1" s="4">
         <f>SUM($D:$D)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N1" s="7">
         <f>N2/L1</f>
-        <v>0.8571428571428571</v>
+        <v>0.86046511627906974</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,32 +808,32 @@
       </c>
       <c r="B2" s="9">
         <f>[1]Sheet1!$H$2</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="9">
         <f>[1]Sheet1!$H$3</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="9">
         <f>[1]Sheet1!$H$1</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="19">
         <f t="shared" ref="E2" si="0">C2/D2</f>
-        <v>0.5714285714285714</v>
+        <v>0.62068965517241381</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="12">
         <f>[1]Sheet1!$H$6</f>
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="H2" s="9">
         <f>[1]Sheet1!$H$5</f>
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="I2" s="22">
         <f t="shared" ref="I2" si="1">G2/H2</f>
-        <v>0.568075117370892</v>
+        <v>0.62995594713656389</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="4" t="s">
@@ -841,14 +841,14 @@
       </c>
       <c r="L2" s="4">
         <f>SUM($B:$B)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="3">
         <f>SUM(L2:L3)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -890,21 +890,21 @@
       </c>
       <c r="L3" s="4">
         <f>SUM($C:$C)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="7">
         <f>L3/L1</f>
-        <v>0.5714285714285714</v>
+        <v>0.60465116279069764</v>
       </c>
       <c r="O3" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="24">
         <f>L3/N2</f>
-        <v>0.66666666666666663</v>
+        <v>0.70270270270270274</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="12">
         <f>[4]Sheet1!$G$5</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="9">
         <f>[4]Sheet1!$G$4</f>
@@ -976,7 +976,7 @@
       </c>
       <c r="I5" s="22">
         <f t="shared" ref="I5" si="3">G5/H5</f>
-        <v>0.18518518518518517</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="4" t="s">
@@ -984,7 +984,7 @@
       </c>
       <c r="L5" s="4">
         <f xml:space="preserve"> SUM($H:$H)</f>
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L6" s="4">
         <f xml:space="preserve"> SUM($G:$G)</f>
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="L7" s="7">
         <f>L6/L5</f>
-        <v>0.55555555555555558</v>
+        <v>0.59687500000000004</v>
       </c>
       <c r="M7" s="3"/>
     </row>

</xml_diff>

<commit_message>
REFACTOR: Updates for Completed with Errors story
</commit_message>
<xml_diff>
--- a/QA/Tests/_Test_Suite_Total_Statistics.xlsx
+++ b/QA/Tests/_Test_Suite_Total_Statistics.xlsx
@@ -381,10 +381,10 @@
       <sheetData sheetId="0">
         <row r="1">
           <cell r="E1">
-            <v>5</v>
+            <v>7</v>
           </cell>
           <cell r="G1">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="2">
@@ -394,7 +394,7 @@
         </row>
         <row r="4">
           <cell r="G4">
-            <v>25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="5">
@@ -837,14 +837,14 @@
       </c>
       <c r="L1" s="4">
         <f>SUM($D:$D)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N1" s="7">
         <f>N2/L1</f>
-        <v>0.79032258064516125</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,14 +886,14 @@
       </c>
       <c r="L2" s="4">
         <f>SUM($B:$B)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="3">
         <f>SUM(L2:L3)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -942,14 +942,14 @@
       </c>
       <c r="N3" s="7">
         <f>L3/L1</f>
-        <v>0.69354838709677424</v>
+        <v>0.671875</v>
       </c>
       <c r="O3" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="24">
         <f>L3/N2</f>
-        <v>0.87755102040816324</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
       </c>
       <c r="B4" s="9">
         <f>[3]Sheet1!$G$1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="9">
         <f>[3]Sheet1!$G$2</f>
@@ -966,11 +966,11 @@
       </c>
       <c r="D4" s="9">
         <f>[3]Sheet1!$E$1</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="19">
         <f>C4/D4</f>
-        <v>0.6</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="12">
@@ -979,11 +979,11 @@
       </c>
       <c r="H4" s="9">
         <f>[3]Sheet1!$G$4</f>
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="I4" s="22">
         <f>G4/H4</f>
-        <v>0.64</v>
+        <v>0.43243243243243246</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="4"/>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="L5" s="4">
         <f xml:space="preserve"> SUM($H:$H)</f>
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="L7" s="7">
         <f>L6/L5</f>
-        <v>0.73483146067415728</v>
+        <v>0.71553610503282272</v>
       </c>
       <c r="M7" s="3"/>
     </row>

</xml_diff>